<commit_message>
FINFLUX-2789 Correcting Failed Overdue scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/2495-RBI-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-DATE-VAR-INST-PERIODIC-Makerepayment2.xlsx
+++ b/Finflux Automation Excels/Client/2495-RBI-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-DATE-VAR-INST-PERIODIC-Makerepayment2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\finflux_automation_test\Finflux Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="816" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="816" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -154,8 +159,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +181,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -225,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -263,17 +281,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -283,6 +304,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -331,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,9 +388,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,6 +440,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1019,132 +1077,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="20" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="21">
         <v>151</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22">
         <v>42050</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="21">
         <v>152</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="22">
         <v>42050</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="21">
         <v>154</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="22">
         <v>42050</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1330,11 +1386,11 @@
       <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1357,11 +1413,11 @@
       <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1384,13 +1440,13 @@
       <c r="F4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="17"/>
+      <c r="I4" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1401,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,35 +1474,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>27</v>
       </c>
@@ -1468,12 +1524,12 @@
       <c r="G2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>28</v>
       </c>
@@ -1495,21 +1551,21 @@
       <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1533,10 +1589,10 @@
       <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -1560,21 +1616,21 @@
       <c r="G6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -1598,10 +1654,10 @@
       <c r="G8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1625,8 +1681,8 @@
       <c r="G9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>